<commit_message>
Update cover in the remaining scenario files
</commit_message>
<xml_diff>
--- a/SuppXLS/Scen_B_IND_Emi_Proc.xlsx
+++ b/SuppXLS/Scen_B_IND_Emi_Proc.xlsx
@@ -8,18 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Olex\Documents\MANRID\ResLab\Modelling\TIMES\TIMES-IE\SuppXLS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD0E0358-250A-43E9-83C1-5C086A5476A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85DCF4D2-C72B-40FE-BB1D-9730C48BF606}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Cover" sheetId="12" r:id="rId1"/>
     <sheet name="Regions" sheetId="2" r:id="rId2"/>
     <sheet name="Emissions" sheetId="11" r:id="rId3"/>
   </sheets>
-  <externalReferences>
-    <externalReference r:id="rId4"/>
-  </externalReferences>
   <definedNames>
     <definedName name="__123Graph_AEUMILKPN" localSheetId="0" hidden="1">#REF!</definedName>
     <definedName name="__123Graph_AEUMILKPN" hidden="1">#REF!</definedName>
@@ -143,7 +140,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="510" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="511" uniqueCount="95">
   <si>
     <t>Development</t>
   </si>
@@ -403,27 +400,15 @@
     <t>Document type:</t>
   </si>
   <si>
-    <t>Template type</t>
-  </si>
-  <si>
     <t>Sector(s):</t>
   </si>
   <si>
-    <t>Sector name</t>
-  </si>
-  <si>
     <t>Purpose:</t>
   </si>
   <si>
-    <t>Brief description of what this file is for</t>
-  </si>
-  <si>
     <t>Original developer(s):</t>
   </si>
   <si>
-    <t>Full Name(s) (Affiliation, email)</t>
-  </si>
-  <si>
     <t>Current maintainer(s):</t>
   </si>
   <si>
@@ -443,6 +428,21 @@
   </si>
   <si>
     <t>https://creativecommons.org/licenses/by-nc-sa/4.0/</t>
+  </si>
+  <si>
+    <t>Scenario</t>
+  </si>
+  <si>
+    <t>Olexandr Balyk (UCC, olexandr.balyk@ucc.ie)</t>
+  </si>
+  <si>
+    <t>Industry sector (IND)</t>
+  </si>
+  <si>
+    <t>Specify process emissions</t>
+  </si>
+  <si>
+    <t>Ankita Gaur (UCC, agaur@ucc.ie)</t>
   </si>
 </sst>
 </file>
@@ -799,9 +799,6 @@
     <xf numFmtId="0" fontId="9" fillId="10" borderId="0" xfId="3" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="9" borderId="0" xfId="3" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="11" fillId="10" borderId="0" xfId="3" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -820,9 +817,6 @@
     <xf numFmtId="0" fontId="14" fillId="9" borderId="0" xfId="3" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="9" borderId="0" xfId="3" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="15" fillId="10" borderId="0" xfId="3" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -835,14 +829,20 @@
     <xf numFmtId="165" fontId="15" fillId="9" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="9" borderId="0" xfId="2" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="17" fillId="10" borderId="0" xfId="3" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="9" borderId="0" xfId="3" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="9" borderId="0" xfId="2" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="9" borderId="0" xfId="3" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="9" borderId="0" xfId="3" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="9" borderId="0" xfId="2" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1205,7 +1205,7 @@
                   <a14:compatExt spid="_x0000_s1025"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000001040000}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000001040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1241,19 +1241,6 @@
     <mc:Fallback/>
   </mc:AlternateContent>
 </xdr:wsDr>
-</file>
-
-<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
-      <sheetName val="Cover"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0"/>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1523,7 +1510,7 @@
   <dimension ref="A1:Z99"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I10" sqref="I10"/>
+      <selection activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1961,20 +1948,20 @@
       <c r="Z15" s="28"/>
     </row>
     <row r="16" spans="1:26" ht="102.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="29" t="s">
+      <c r="A16" s="43" t="s">
         <v>78</v>
       </c>
-      <c r="B16" s="29"/>
-      <c r="C16" s="29"/>
-      <c r="D16" s="29"/>
-      <c r="E16" s="30"/>
-      <c r="F16" s="30"/>
-      <c r="G16" s="31"/>
-      <c r="H16" s="31"/>
-      <c r="I16" s="31"/>
-      <c r="J16" s="31"/>
-      <c r="K16" s="31"/>
-      <c r="L16" s="31"/>
+      <c r="B16" s="43"/>
+      <c r="C16" s="43"/>
+      <c r="D16" s="43"/>
+      <c r="E16" s="29"/>
+      <c r="F16" s="29"/>
+      <c r="G16" s="30"/>
+      <c r="H16" s="30"/>
+      <c r="I16" s="30"/>
+      <c r="J16" s="30"/>
+      <c r="K16" s="30"/>
+      <c r="L16" s="30"/>
       <c r="M16" s="28"/>
       <c r="N16" s="28"/>
       <c r="O16" s="28"/>
@@ -1991,10 +1978,10 @@
       <c r="Z16" s="28"/>
     </row>
     <row r="17" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="32"/>
-      <c r="B17" s="32"/>
-      <c r="C17" s="32"/>
-      <c r="D17" s="32"/>
+      <c r="A17" s="31"/>
+      <c r="B17" s="31"/>
+      <c r="C17" s="31"/>
+      <c r="D17" s="31"/>
       <c r="E17" s="28"/>
       <c r="F17" s="28"/>
       <c r="G17" s="28"/>
@@ -2019,18 +2006,18 @@
       <c r="Z17" s="28"/>
     </row>
     <row r="18" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="32"/>
-      <c r="B18" s="32"/>
-      <c r="C18" s="32"/>
-      <c r="D18" s="32"/>
-      <c r="E18" s="33"/>
-      <c r="F18" s="33"/>
-      <c r="G18" s="34"/>
-      <c r="H18" s="34"/>
-      <c r="I18" s="34"/>
-      <c r="J18" s="34"/>
-      <c r="K18" s="34"/>
-      <c r="L18" s="34"/>
+      <c r="A18" s="31"/>
+      <c r="B18" s="31"/>
+      <c r="C18" s="31"/>
+      <c r="D18" s="31"/>
+      <c r="E18" s="32"/>
+      <c r="F18" s="32"/>
+      <c r="G18" s="33"/>
+      <c r="H18" s="33"/>
+      <c r="I18" s="33"/>
+      <c r="J18" s="33"/>
+      <c r="K18" s="33"/>
+      <c r="L18" s="33"/>
       <c r="M18" s="28"/>
       <c r="N18" s="28"/>
       <c r="O18" s="28"/>
@@ -2047,22 +2034,22 @@
       <c r="Z18" s="28"/>
     </row>
     <row r="19" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="35" t="s">
+      <c r="A19" s="34" t="s">
         <v>79</v>
       </c>
-      <c r="B19" s="36" t="s">
-        <v>80</v>
-      </c>
-      <c r="C19" s="36"/>
-      <c r="D19" s="36"/>
-      <c r="E19" s="37"/>
-      <c r="F19" s="37"/>
-      <c r="G19" s="38"/>
-      <c r="H19" s="38"/>
-      <c r="I19" s="38"/>
-      <c r="J19" s="38"/>
-      <c r="K19" s="38"/>
-      <c r="L19" s="38"/>
+      <c r="B19" s="42" t="s">
+        <v>90</v>
+      </c>
+      <c r="C19" s="42"/>
+      <c r="D19" s="42"/>
+      <c r="E19" s="35"/>
+      <c r="F19" s="35"/>
+      <c r="G19" s="36"/>
+      <c r="H19" s="36"/>
+      <c r="I19" s="36"/>
+      <c r="J19" s="36"/>
+      <c r="K19" s="36"/>
+      <c r="L19" s="36"/>
       <c r="M19" s="28"/>
       <c r="N19" s="28"/>
       <c r="O19" s="28"/>
@@ -2079,22 +2066,22 @@
       <c r="Z19" s="28"/>
     </row>
     <row r="20" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="35" t="s">
-        <v>81</v>
-      </c>
-      <c r="B20" s="36" t="s">
-        <v>82</v>
-      </c>
-      <c r="C20" s="36"/>
-      <c r="D20" s="36"/>
-      <c r="E20" s="37"/>
-      <c r="F20" s="37"/>
-      <c r="G20" s="38"/>
-      <c r="H20" s="38"/>
-      <c r="I20" s="38"/>
-      <c r="J20" s="38"/>
-      <c r="K20" s="38"/>
-      <c r="L20" s="38"/>
+      <c r="A20" s="34" t="s">
+        <v>80</v>
+      </c>
+      <c r="B20" s="42" t="s">
+        <v>92</v>
+      </c>
+      <c r="C20" s="42"/>
+      <c r="D20" s="42"/>
+      <c r="E20" s="35"/>
+      <c r="F20" s="35"/>
+      <c r="G20" s="36"/>
+      <c r="H20" s="36"/>
+      <c r="I20" s="36"/>
+      <c r="J20" s="36"/>
+      <c r="K20" s="36"/>
+      <c r="L20" s="36"/>
       <c r="M20" s="28"/>
       <c r="N20" s="28"/>
       <c r="O20" s="28"/>
@@ -2111,22 +2098,22 @@
       <c r="Z20" s="28"/>
     </row>
     <row r="21" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="35" t="s">
-        <v>83</v>
-      </c>
-      <c r="B21" s="39" t="s">
-        <v>84</v>
-      </c>
-      <c r="C21" s="39"/>
-      <c r="D21" s="39"/>
-      <c r="E21" s="37"/>
-      <c r="F21" s="37"/>
-      <c r="G21" s="38"/>
-      <c r="H21" s="38"/>
-      <c r="I21" s="38"/>
-      <c r="J21" s="38"/>
-      <c r="K21" s="38"/>
-      <c r="L21" s="38"/>
+      <c r="A21" s="34" t="s">
+        <v>81</v>
+      </c>
+      <c r="B21" s="37" t="s">
+        <v>93</v>
+      </c>
+      <c r="C21" s="37"/>
+      <c r="D21" s="37"/>
+      <c r="E21" s="35"/>
+      <c r="F21" s="35"/>
+      <c r="G21" s="36"/>
+      <c r="H21" s="36"/>
+      <c r="I21" s="36"/>
+      <c r="J21" s="36"/>
+      <c r="K21" s="36"/>
+      <c r="L21" s="36"/>
       <c r="M21" s="28"/>
       <c r="N21" s="28"/>
       <c r="O21" s="28"/>
@@ -2143,18 +2130,18 @@
       <c r="Z21" s="28"/>
     </row>
     <row r="22" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="35"/>
-      <c r="B22" s="39"/>
-      <c r="C22" s="39"/>
-      <c r="D22" s="39"/>
-      <c r="E22" s="37"/>
-      <c r="F22" s="37"/>
-      <c r="G22" s="38"/>
-      <c r="H22" s="38"/>
-      <c r="I22" s="38"/>
-      <c r="J22" s="38"/>
-      <c r="K22" s="38"/>
-      <c r="L22" s="38"/>
+      <c r="A22" s="34"/>
+      <c r="B22" s="37"/>
+      <c r="C22" s="37"/>
+      <c r="D22" s="37"/>
+      <c r="E22" s="35"/>
+      <c r="F22" s="35"/>
+      <c r="G22" s="36"/>
+      <c r="H22" s="36"/>
+      <c r="I22" s="36"/>
+      <c r="J22" s="36"/>
+      <c r="K22" s="36"/>
+      <c r="L22" s="36"/>
       <c r="M22" s="28"/>
       <c r="N22" s="28"/>
       <c r="O22" s="28"/>
@@ -2171,14 +2158,14 @@
       <c r="Z22" s="28"/>
     </row>
     <row r="23" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="35" t="s">
-        <v>85</v>
-      </c>
-      <c r="B23" s="36" t="s">
-        <v>86</v>
-      </c>
-      <c r="C23" s="36"/>
-      <c r="D23" s="36"/>
+      <c r="A23" s="34" t="s">
+        <v>82</v>
+      </c>
+      <c r="B23" s="42" t="s">
+        <v>94</v>
+      </c>
+      <c r="C23" s="42"/>
+      <c r="D23" s="42"/>
       <c r="E23" s="28"/>
       <c r="F23" s="28"/>
       <c r="G23" s="28"/>
@@ -2203,10 +2190,10 @@
       <c r="Z23" s="28"/>
     </row>
     <row r="24" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="35"/>
-      <c r="B24" s="39"/>
-      <c r="C24" s="39"/>
-      <c r="D24" s="39"/>
+      <c r="A24" s="34"/>
+      <c r="B24" s="37"/>
+      <c r="C24" s="37"/>
+      <c r="D24" s="37"/>
       <c r="E24" s="28"/>
       <c r="F24" s="28"/>
       <c r="G24" s="28"/>
@@ -2231,10 +2218,10 @@
       <c r="Z24" s="28"/>
     </row>
     <row r="25" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="35"/>
-      <c r="B25" s="39"/>
-      <c r="C25" s="39"/>
-      <c r="D25" s="39"/>
+      <c r="A25" s="34"/>
+      <c r="B25" s="37"/>
+      <c r="C25" s="37"/>
+      <c r="D25" s="37"/>
       <c r="E25" s="28"/>
       <c r="F25" s="28"/>
       <c r="G25" s="28"/>
@@ -2259,14 +2246,14 @@
       <c r="Z25" s="28"/>
     </row>
     <row r="26" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="35" t="s">
-        <v>87</v>
-      </c>
-      <c r="B26" s="36" t="s">
-        <v>86</v>
-      </c>
-      <c r="C26" s="36"/>
-      <c r="D26" s="36"/>
+      <c r="A26" s="34" t="s">
+        <v>83</v>
+      </c>
+      <c r="B26" s="42" t="s">
+        <v>94</v>
+      </c>
+      <c r="C26" s="42"/>
+      <c r="D26" s="42"/>
       <c r="E26" s="28"/>
       <c r="F26" s="28"/>
       <c r="G26" s="28"/>
@@ -2291,10 +2278,12 @@
       <c r="Z26" s="28"/>
     </row>
     <row r="27" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="35"/>
-      <c r="B27" s="39"/>
-      <c r="C27" s="39"/>
-      <c r="D27" s="39"/>
+      <c r="A27" s="34"/>
+      <c r="B27" s="37" t="s">
+        <v>91</v>
+      </c>
+      <c r="C27" s="37"/>
+      <c r="D27" s="37"/>
       <c r="E27" s="28"/>
       <c r="F27" s="28"/>
       <c r="G27" s="28"/>
@@ -2319,10 +2308,10 @@
       <c r="Z27" s="28"/>
     </row>
     <row r="28" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="35"/>
-      <c r="B28" s="39"/>
-      <c r="C28" s="39"/>
-      <c r="D28" s="39"/>
+      <c r="A28" s="34"/>
+      <c r="B28" s="37"/>
+      <c r="C28" s="37"/>
+      <c r="D28" s="37"/>
       <c r="E28" s="28"/>
       <c r="F28" s="28"/>
       <c r="G28" s="28"/>
@@ -2347,14 +2336,14 @@
       <c r="Z28" s="28"/>
     </row>
     <row r="29" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="35" t="s">
-        <v>88</v>
-      </c>
-      <c r="B29" s="40">
+      <c r="A29" s="34" t="s">
+        <v>84</v>
+      </c>
+      <c r="B29" s="38">
         <v>1</v>
       </c>
-      <c r="C29" s="39"/>
-      <c r="D29" s="39"/>
+      <c r="C29" s="37"/>
+      <c r="D29" s="37"/>
       <c r="E29" s="28"/>
       <c r="F29" s="28"/>
       <c r="G29" s="28"/>
@@ -2379,16 +2368,16 @@
       <c r="Z29" s="28"/>
     </row>
     <row r="30" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="35" t="s">
-        <v>89</v>
-      </c>
-      <c r="B30" s="41" t="s">
-        <v>90</v>
-      </c>
-      <c r="C30" s="36"/>
-      <c r="D30" s="36"/>
-      <c r="E30" s="42"/>
-      <c r="F30" s="42"/>
+      <c r="A30" s="34" t="s">
+        <v>85</v>
+      </c>
+      <c r="B30" s="44" t="s">
+        <v>86</v>
+      </c>
+      <c r="C30" s="42"/>
+      <c r="D30" s="42"/>
+      <c r="E30" s="39"/>
+      <c r="F30" s="39"/>
       <c r="G30" s="28"/>
       <c r="H30" s="28"/>
       <c r="I30" s="28"/>
@@ -2411,16 +2400,16 @@
       <c r="Z30" s="28"/>
     </row>
     <row r="31" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="35" t="s">
-        <v>91</v>
-      </c>
-      <c r="B31" s="36" t="s">
-        <v>92</v>
-      </c>
-      <c r="C31" s="36"/>
-      <c r="D31" s="36"/>
-      <c r="E31" s="42"/>
-      <c r="F31" s="42"/>
+      <c r="A31" s="34" t="s">
+        <v>87</v>
+      </c>
+      <c r="B31" s="42" t="s">
+        <v>88</v>
+      </c>
+      <c r="C31" s="42"/>
+      <c r="D31" s="42"/>
+      <c r="E31" s="39"/>
+      <c r="F31" s="39"/>
       <c r="G31" s="28"/>
       <c r="H31" s="28"/>
       <c r="I31" s="28"/>
@@ -2443,12 +2432,12 @@
       <c r="Z31" s="28"/>
     </row>
     <row r="32" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="43"/>
-      <c r="B32" s="44" t="s">
-        <v>93</v>
-      </c>
-      <c r="C32" s="43"/>
-      <c r="D32" s="43"/>
+      <c r="A32" s="40"/>
+      <c r="B32" s="41" t="s">
+        <v>89</v>
+      </c>
+      <c r="C32" s="40"/>
+      <c r="D32" s="40"/>
       <c r="E32" s="28"/>
       <c r="F32" s="28"/>
       <c r="G32" s="28"/>
@@ -5139,8 +5128,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="B1:O110"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="I68" sqref="I68"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K1" sqref="K1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>